<commit_message>
Excel gestion de cambios, version 1 de la presentacion 3 y matriz RACI
</commit_message>
<xml_diff>
--- a/Gestion_Cambios_V00.xlsx
+++ b/Gestion_Cambios_V00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mari Cortes\Documents\Gestion_P_Github\Gestion_Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{259CB8CC-CF0D-4CCC-B807-A54281A79C58}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{82DB2C26-23FF-48C3-B169-1BA1D0D17098}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{85130BB3-66DA-47C0-B640-E983F215480D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Proyecto</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Reducción de dias</t>
+  </si>
+  <si>
+    <t>Actualización de responsables</t>
+  </si>
+  <si>
+    <t>4.1, 5.3 y 6.3</t>
+  </si>
+  <si>
+    <t>1.2</t>
   </si>
 </sst>
 </file>
@@ -231,24 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -260,6 +251,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,7 +592,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,620 +610,638 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4">
         <v>43403</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4">
         <v>43406</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="8"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4">
         <v>43406</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4">
         <v>43408</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="8"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
         <v>43412</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="8"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4">
         <v>43418</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43419</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Añadidas animaciones a Presentación3.pptx y ajuste de duración de actividades en el DICCIONARIO DE LA WBS.docx.
</commit_message>
<xml_diff>
--- a/Gestion_Cambios_V00.xlsx
+++ b/Gestion_Cambios_V00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mari Cortes\Documents\Gestion_P_Github\Gestion_Proyectos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GalleDoh\Documents\GESTION_PROY_REPO\Gestion_Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{82DB2C26-23FF-48C3-B169-1BA1D0D17098}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B4A494-E7A2-4747-B791-C156EDF3B998}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{85130BB3-66DA-47C0-B640-E983F215480D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
   <si>
     <t>Proyecto</t>
   </si>
@@ -148,6 +148,30 @@
   </si>
   <si>
     <t>1.2</t>
+  </si>
+  <si>
+    <t>16/11/2018</t>
+  </si>
+  <si>
+    <t>Dpo.Control y calidad</t>
+  </si>
+  <si>
+    <t>Modificación Gestión del Tiempo</t>
+  </si>
+  <si>
+    <t>17/11/2018</t>
+  </si>
+  <si>
+    <t>Adición de información</t>
+  </si>
+  <si>
+    <t>18/11/2018</t>
+  </si>
+  <si>
+    <t>2.1,3.1</t>
+  </si>
+  <si>
+    <t>Cambio duración de tareas</t>
   </si>
 </sst>
 </file>
@@ -293,7 +317,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -592,16 +616,17 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="50.42578125" bestFit="1" customWidth="1"/>
@@ -711,7 +736,7 @@
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -789,10 +814,10 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="4">
@@ -828,10 +853,10 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4">
@@ -867,10 +892,10 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="4">
@@ -900,14 +925,14 @@
       <c r="K8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="4">
@@ -931,241 +956,303 @@
       <c r="I9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="J9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1178,9 +1265,9 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1193,9 +1280,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1208,7 +1295,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>

</xml_diff>

<commit_message>
Añadida entrada en gestión de cambios.
</commit_message>
<xml_diff>
--- a/Gestion_Cambios_V00.xlsx
+++ b/Gestion_Cambios_V00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mari Cortes\Documents\Gestion_P_Github\Gestion_Proyectos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GalleDoh\Documents\GESTION_PROY_REPO\Gestion_Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{82DB2C26-23FF-48C3-B169-1BA1D0D17098}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56B8E56-0BF3-45D1-B74C-E993CB99232E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{85130BB3-66DA-47C0-B640-E983F215480D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
   <si>
     <t>Proyecto</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>1.2</t>
+  </si>
+  <si>
+    <t>Correción y adición de mapas de procesos a E_3</t>
+  </si>
+  <si>
+    <t>Anexo RRHH1 y 2</t>
+  </si>
+  <si>
+    <t>Nuevos mapas de procesos, corrección en el uso de referencias</t>
   </si>
 </sst>
 </file>
@@ -293,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -592,10 +601,10 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -708,7 +717,9 @@
       <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -747,7 +758,9 @@
       <c r="L4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="2"/>
+      <c r="M4" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -786,7 +799,9 @@
       <c r="L5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -825,7 +840,9 @@
       <c r="L6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="2"/>
+      <c r="M6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -864,7 +881,9 @@
       <c r="L7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -901,7 +920,9 @@
         <v>37</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="M8" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -931,14 +952,16 @@
       <c r="I9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="2"/>
+      <c r="L9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -947,17 +970,37 @@
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="2"/>
+      <c r="C10" s="4">
+        <v>43428</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">

</xml_diff>

<commit_message>
Memoria Gestion COMMS y Riesgos.
</commit_message>
<xml_diff>
--- a/Gestion_Cambios_V00.xlsx
+++ b/Gestion_Cambios_V00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GalleDoh\Documents\GESTION_PROY_REPO\Gestion_Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56B8E56-0BF3-45D1-B74C-E993CB99232E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB230262-1362-4B68-A90D-D043A622669D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{85130BB3-66DA-47C0-B640-E983F215480D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="53">
   <si>
     <t>Proyecto</t>
   </si>
@@ -157,6 +157,33 @@
   </si>
   <si>
     <t>Nuevos mapas de procesos, corrección en el uso de referencias</t>
+  </si>
+  <si>
+    <t>Aceptación del documento de Gestión de las COMMS y Riegos.</t>
+  </si>
+  <si>
+    <t>3,4,5</t>
+  </si>
+  <si>
+    <t>Necesidad de un Plan de Gestión de COMMS y Riesgos</t>
+  </si>
+  <si>
+    <t>Dpto.ctrl y Calidad</t>
+  </si>
+  <si>
+    <t>Modificación de la clasificación de riesgos.</t>
+  </si>
+  <si>
+    <t>Mejora de la caracterización y planificación de riesgos</t>
+  </si>
+  <si>
+    <t>Dpto.Control y Calidad</t>
+  </si>
+  <si>
+    <t>Modificación colores de la matriz de probabilidad e impacto.</t>
+  </si>
+  <si>
+    <t>Mejora de los colores elegidos para la matriz de probabilidad e impacto.</t>
   </si>
 </sst>
 </file>
@@ -244,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +287,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,7 +631,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="M13" activeCellId="5" sqref="H13 H12 J13 K13 L13 M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,25 +649,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="6" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1009,17 +1039,39 @@
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="C11" s="6">
+        <v>43442</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="3">
+        <v>13</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1028,17 +1080,39 @@
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="C12" s="6">
+        <v>43445</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1047,17 +1121,39 @@
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="C13" s="4">
+        <v>43446</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
Correcciones mínimas y actualización del documento de cambios.
</commit_message>
<xml_diff>
--- a/Gestion_Cambios_V00.xlsx
+++ b/Gestion_Cambios_V00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GalleDoh\Documents\GESTION_PROY_REPO\Gestion_Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB230262-1362-4B68-A90D-D043A622669D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76CAD5E-3E87-4027-8C53-23445412760C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{85130BB3-66DA-47C0-B640-E983F215480D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="60">
   <si>
     <t>Proyecto</t>
   </si>
@@ -184,6 +184,27 @@
   </si>
   <si>
     <t>Mejora de los colores elegidos para la matriz de probabilidad e impacto.</t>
+  </si>
+  <si>
+    <t>15/12/2018</t>
+  </si>
+  <si>
+    <t>Creación G.Costes y Justificación</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>23/12/2018</t>
+  </si>
+  <si>
+    <t>24/12/2018</t>
+  </si>
+  <si>
+    <t>Correción documento costes</t>
+  </si>
+  <si>
+    <t>Adición jutificación</t>
   </si>
 </sst>
 </file>
@@ -631,7 +652,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" activeCellId="5" sqref="H13 H12 J13 K13 L13 M13"/>
+      <selection activeCell="J15" sqref="J15:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,17 +1183,39 @@
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1181,17 +1224,39 @@
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1200,17 +1265,39 @@
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">

</xml_diff>

<commit_message>
Añadidos los cambios del documento final
</commit_message>
<xml_diff>
--- a/Gestion_Cambios_V00.xlsx
+++ b/Gestion_Cambios_V00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GalleDoh\Documents\GESTION_PROY_REPO\Gestion_Proyectos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mari Cortes\Documents\Gestion_P_Github\Gestion_Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76CAD5E-3E87-4027-8C53-23445412760C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBF76D-1A3C-4D64-9229-57CA15010F55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{85130BB3-66DA-47C0-B640-E983F215480D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="64">
   <si>
     <t>Proyecto</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>Adición jutificación</t>
+  </si>
+  <si>
+    <t>Realización de doc.final</t>
+  </si>
+  <si>
+    <t>Añadido de documentación</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
   </si>
 </sst>
 </file>
@@ -292,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,9 +320,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,7 +362,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -652,17 +661,17 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:M16"/>
+      <selection activeCell="C3" sqref="C3:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
@@ -670,25 +679,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="7" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1036,7 +1045,7 @@
       <c r="G10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1060,7 +1069,7 @@
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>43442</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1075,7 +1084,7 @@
       <c r="G11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>45</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1101,7 +1110,7 @@
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>43445</v>
       </c>
       <c r="D12" s="3">
@@ -1186,10 +1195,10 @@
       <c r="C14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -1198,7 +1207,7 @@
       <c r="G14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>55</v>
       </c>
       <c r="I14" s="5" t="s">
@@ -1239,7 +1248,7 @@
       <c r="G15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>55</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -1280,7 +1289,7 @@
       <c r="G16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>55</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -1306,13 +1315,27 @@
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="C17" s="4">
+        <v>43474</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1325,13 +1348,27 @@
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="C18" s="4">
+        <v>43480</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1344,25 +1381,35 @@
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="C19" s="4">
+        <v>43484</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1376,12 +1423,8 @@
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="3"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>

</xml_diff>